<commit_message>
Pre-RIF commit. Mostly scripts for PSMC and ROH analyses.
</commit_message>
<xml_diff>
--- a/data-raw/lcWGS.final.sample.list.allspecies.xlsx
+++ b/data-raw/lcWGS.final.sample.list.allspecies.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Shared/KKMDocuments/Documents/Github.Repos/Multi-species-GTseq/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ABEC98E-FAC7-FB4C-8844-25030A0C2DA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3440F194-3CE0-F545-8243-660694402D60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2500" yWindow="7380" windowWidth="30240" windowHeight="18880" activeTab="1" xr2:uid="{84B52217-D092-8E49-BE00-5F1ADCA94243}"/>
+    <workbookView xWindow="2500" yWindow="7380" windowWidth="30240" windowHeight="18880" xr2:uid="{84B52217-D092-8E49-BE00-5F1ADCA94243}"/>
   </bookViews>
   <sheets>
     <sheet name="FKWs" sheetId="2" r:id="rId1"/>
@@ -4417,7 +4417,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44E2FFEE-42EF-7149-B469-628B3BA30032}">
   <dimension ref="A1:AD68"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A65" sqref="A65:XFD65"/>
@@ -9889,7 +9889,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08FD1BDF-B0F1-CF4C-99DE-BD885AB56E03}">
   <dimension ref="A1:V39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F27" sqref="F27"/>
     </sheetView>
@@ -12232,13 +12232,13 @@
   <dimension ref="A1:AA26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="V22" sqref="V22"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="14.1640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="9" width="0" hidden="1" customWidth="1"/>
+    <col min="5" max="9" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.2">
@@ -14225,13 +14225,13 @@
   <dimension ref="A1:AC26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="X10" sqref="X10:X26"/>
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="14.1640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="11" width="0" hidden="1" customWidth="1"/>
+    <col min="5" max="11" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.2">

</xml_diff>